<commit_message>
add verify rule scenario
</commit_message>
<xml_diff>
--- a/監視設定チェックシート_Getperf.xlsx
+++ b/監視設定チェックシート_Getperf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="チェック対象" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>* 5行目、D列以降のセルに検査対象サーバ接続情報を入力してください。'server_name'と'platform'は必須です。</t>
   </si>
@@ -116,18 +116,10 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>SSLクライアント証明書の有効期限。getperfctl setup済の場合、有効期限を取得(有効期限は1年間で自動的に更新される)</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>data_transfer</t>
   </si>
   <si>
     <t>データ転送状態</t>
-  </si>
-  <si>
-    <t>エージェントからデータ転送された最新の日付。空白となる場合、日付が古い場合はエージェントからの通信ができない状態になっている</t>
-    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>監視エージェントのサーバ名</t>
@@ -180,27 +172,76 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>domain.VM</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>domain.Windows</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>domain.Storage</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>domain.Oracle</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>domain.Host</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>ostrich</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>paas</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>analysis</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>test_a1</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>domain.MyApps</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>domain.Process</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>転送済みデータを集計した最新の日付。空白もしくは、日付が古い場合はデータ集計ができない状態になっている</t>
+    <rPh sb="0" eb="2">
+      <t>テンソウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シュウケイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>シュウケイ</t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>エージェントからデータ転送された最新の日付。空白もしくは、日付が古い場合はエージェントからの通信ができない状態になっている</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>SSLクライアント証明書の有効期限内か。getperfctl setup済の場合、有効期限が取得できる。有効期限は1年毎に自動的に更新される。旧エージェントの場合は、SSL有効期限の設定はなく、Unkownとなる</t>
+    <rPh sb="17" eb="18">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ゴト</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>キュウ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>キゲン</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>セッテイ</t>
+    </rPh>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -667,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -768,12 +809,14 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="4"/>
@@ -788,12 +831,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -808,12 +853,14 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -828,12 +875,14 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -848,13 +897,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>D5</f>
-        <v>ostrich</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>paas</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f>E5</f>
+        <v>test_a1</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -996,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1056,7 +1108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1073,7 +1125,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
@@ -1081,10 +1133,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
@@ -1093,35 +1145,37 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -1129,11 +1183,11 @@
     <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
@@ -1141,11 +1195,11 @@
     <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
@@ -1153,36 +1207,28 @@
     <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
-      <c r="B12" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
     </row>
@@ -1663,10 +1709,10 @@
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>

</xml_diff>